<commit_message>
Refactored Evaluation Collapsing and Lua Scripts
</commit_message>
<xml_diff>
--- a/examples/eop_config/spreadsheets/example-classroom_seating_plan-org.xlsx
+++ b/examples/eop_config/spreadsheets/example-classroom_seating_plan-org.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Programming\cpp\entity_organisation_program\examples\eop_config\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE05141-8F6E-4682-9399-1A30D57E06E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C553AFEC-721F-4816-ADA9-0CBEE45EDDD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
   <si>
     <t/>
   </si>
@@ -97,169 +97,145 @@
     <t>Organisation of Entities: seating_plan_maths</t>
   </si>
   <si>
-    <t>Brooke Layton, maths</t>
-  </si>
-  <si>
-    <t>James Eilbeck, maths</t>
-  </si>
-  <si>
-    <t>Benjamin Hillary, maths</t>
-  </si>
-  <si>
-    <t>Caitlin Boyd, maths</t>
-  </si>
-  <si>
-    <t>Thomas Barrett, maths</t>
-  </si>
-  <si>
-    <t>Samuel Dixon, maths</t>
-  </si>
-  <si>
-    <t>Matthew Homan, maths</t>
-  </si>
-  <si>
-    <t>James Calderon, maths</t>
-  </si>
-  <si>
-    <t>Ruby Haigh, maths</t>
-  </si>
-  <si>
-    <t>Nancy Enyoazu, maths</t>
-  </si>
-  <si>
-    <t>Benedict Hobday, maths</t>
-  </si>
-  <si>
-    <t>Stanley Hirst, maths</t>
-  </si>
-  <si>
-    <t>Alex Sentance, maths</t>
-  </si>
-  <si>
-    <t>Katrina Petersone, maths</t>
-  </si>
-  <si>
-    <t>Benjamin Finn, maths</t>
-  </si>
-  <si>
-    <t>Madison Taylor, maths</t>
-  </si>
-  <si>
-    <t>Lexi Green, maths</t>
-  </si>
-  <si>
-    <t>Spencer Rowe, maths</t>
-  </si>
-  <si>
-    <t>Sophie Rayner, maths</t>
-  </si>
-  <si>
-    <t>Esther Sido, maths</t>
-  </si>
-  <si>
-    <t>James Shilton, maths</t>
-  </si>
-  <si>
-    <t>Niko Morris, maths</t>
-  </si>
-  <si>
-    <t>William Hunt, maths</t>
-  </si>
-  <si>
-    <t>Violet Hudson, maths</t>
-  </si>
-  <si>
-    <t>Aarron Kelly, maths</t>
-  </si>
-  <si>
-    <t>Ava Lee, maths</t>
-  </si>
-  <si>
     <t>Organisation of Entities: seating_plan_english</t>
   </si>
   <si>
-    <t>Lexie Starkey, english</t>
-  </si>
-  <si>
-    <t>Matthew Homan, english</t>
-  </si>
-  <si>
-    <t>Niamh Teale, english</t>
-  </si>
-  <si>
-    <t>James Eilbeck, english</t>
-  </si>
-  <si>
-    <t>Cassie Strachan, english</t>
-  </si>
-  <si>
-    <t>Elliott Long, english</t>
-  </si>
-  <si>
-    <t>Caitlin Boyd, english</t>
-  </si>
-  <si>
-    <t>Eva Redican, english</t>
-  </si>
-  <si>
-    <t>Alex Sentance, english</t>
-  </si>
-  <si>
-    <t>Cheryl Kanyimo, english</t>
-  </si>
-  <si>
-    <t>Bethany Greer, english</t>
-  </si>
-  <si>
-    <t>Mariam Keita, english</t>
-  </si>
-  <si>
-    <t>Aarron Kelly, english</t>
-  </si>
-  <si>
-    <t>Lucy Webster, english</t>
-  </si>
-  <si>
-    <t>Hugo Bird, english</t>
-  </si>
-  <si>
-    <t>Samuel Dixon, english</t>
-  </si>
-  <si>
-    <t>Jayden Parsons, english</t>
-  </si>
-  <si>
-    <t>Ethan Durham, english</t>
-  </si>
-  <si>
-    <t>Callum Foster, english</t>
-  </si>
-  <si>
-    <t>Jayden Nasa-Mereni, english</t>
-  </si>
-  <si>
-    <t>James Calderon, english</t>
-  </si>
-  <si>
-    <t>Patryk Rudnicki, english</t>
-  </si>
-  <si>
-    <t>Jude Fitzsimons, english</t>
-  </si>
-  <si>
-    <t>Isabella Holmes, english</t>
-  </si>
-  <si>
-    <t>Lewis Dacre, english</t>
-  </si>
-  <si>
-    <t>Ava Lee, english</t>
-  </si>
-  <si>
     <t>seating_plan_maths</t>
   </si>
   <si>
     <t>seating_plan_english</t>
+  </si>
+  <si>
+    <t>Niko Morris</t>
+  </si>
+  <si>
+    <t>James Eilbeck</t>
+  </si>
+  <si>
+    <t>James Shilton</t>
+  </si>
+  <si>
+    <t>Caitlin Boyd</t>
+  </si>
+  <si>
+    <t>James Calderon</t>
+  </si>
+  <si>
+    <t>Violet Hudson</t>
+  </si>
+  <si>
+    <t>Matthew Homan</t>
+  </si>
+  <si>
+    <t>Stanley Hirst</t>
+  </si>
+  <si>
+    <t>Esther Sido</t>
+  </si>
+  <si>
+    <t>Katrina Petersone</t>
+  </si>
+  <si>
+    <t>Nancy Enyoazu</t>
+  </si>
+  <si>
+    <t>Aarron Kelly</t>
+  </si>
+  <si>
+    <t>William Hunt</t>
+  </si>
+  <si>
+    <t>Thomas Barrett</t>
+  </si>
+  <si>
+    <t>Samuel Dixon</t>
+  </si>
+  <si>
+    <t>Ruby Haigh</t>
+  </si>
+  <si>
+    <t>Benjamin Finn</t>
+  </si>
+  <si>
+    <t>Spencer Rowe</t>
+  </si>
+  <si>
+    <t>Sophie Rayner</t>
+  </si>
+  <si>
+    <t>Lexi Green</t>
+  </si>
+  <si>
+    <t>Brooke Layton</t>
+  </si>
+  <si>
+    <t>Alex Sentance</t>
+  </si>
+  <si>
+    <t>Ava Lee</t>
+  </si>
+  <si>
+    <t>Madison Taylor</t>
+  </si>
+  <si>
+    <t>Benedict Hobday</t>
+  </si>
+  <si>
+    <t>Benjamin Hillary</t>
+  </si>
+  <si>
+    <t>Jayden Parsons</t>
+  </si>
+  <si>
+    <t>Bethany Greer</t>
+  </si>
+  <si>
+    <t>Callum Foster</t>
+  </si>
+  <si>
+    <t>Isabella Holmes</t>
+  </si>
+  <si>
+    <t>Lucy Webster</t>
+  </si>
+  <si>
+    <t>Niamh Teale</t>
+  </si>
+  <si>
+    <t>Ethan Durham</t>
+  </si>
+  <si>
+    <t>Patryk Rudnicki</t>
+  </si>
+  <si>
+    <t>Lexie Starkey</t>
+  </si>
+  <si>
+    <t>Lewis Dacre</t>
+  </si>
+  <si>
+    <t>Cassie Strachan</t>
+  </si>
+  <si>
+    <t>Mariam Keita</t>
+  </si>
+  <si>
+    <t>Cheryl Kanyimo</t>
+  </si>
+  <si>
+    <t>Elliott Long</t>
+  </si>
+  <si>
+    <t>Jayden Nasa-Mereni</t>
+  </si>
+  <si>
+    <t>Jude Fitzsimons</t>
+  </si>
+  <si>
+    <t>Hugo Bird</t>
+  </si>
+  <si>
+    <t>Eva Redican</t>
   </si>
 </sst>
 </file>
@@ -312,14 +288,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,37 +620,37 @@
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="4"/>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>21</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -777,118 +753,118 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="H2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="H2" s="6" t="s">
+      <c r="E3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="C4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="F4" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="4" t="s">
         <v>0</v>
       </c>
     </row>
@@ -911,112 +887,112 @@
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="A1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="F3" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="H4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="4" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>